<commit_message>
adding tests for ticket OCEPROJECT-4941 sub-task of OCEPROJECT-4846
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\wcms-qa-testing-framework\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{723C3CF2-87E1-42AA-AC41-318ECF00D633}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
     <sheet name="R4R" sheetId="3" r:id="rId3"/>
-    <sheet name="SitewideSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>Age</t>
   </si>
@@ -300,24 +300,6 @@
   </si>
   <si>
     <t>Statistics</t>
-  </si>
-  <si>
-    <t>Keyword1</t>
-  </si>
-  <si>
-    <t>Keyword2</t>
-  </si>
-  <si>
-    <t>small cell lung cancer</t>
-  </si>
-  <si>
-    <t>Pancreas</t>
-  </si>
-  <si>
-    <t>pancreatic ductal adenocarcinoma</t>
-  </si>
-  <si>
-    <t>mammography</t>
   </si>
   <si>
     <t>xTerminologyx</t>
@@ -326,7 +308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -752,7 +734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -815,7 +797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1137,7 +1119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1192,7 +1174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
@@ -1202,55 +1184,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>